<commit_message>
fix/enum: updated output.xlsx | changed NOT-SETTLED TO NOT_SETTLED
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahi/Developer/ONDC-NTS-Specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C98283-1600-A042-8B96-7554B475E52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9384C-F062-4741-B3A9-6381BD2F36F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settle_misc" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>message.settlement.orders.provider.status</t>
   </si>
   <si>
-    <t>NOT-SETTLED</t>
-  </si>
-  <si>
     <t>message.settlement.orders.provider.reference_no</t>
   </si>
   <si>
@@ -672,6 +669,9 @@
   </si>
   <si>
     <t>2024-05-09</t>
+  </si>
+  <si>
+    <t>NOT_SETTLED</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1214,7 +1214,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1274,7 +1274,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1294,7 +1294,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1314,7 +1314,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1334,7 +1334,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1354,7 +1354,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1374,7 +1374,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1454,7 +1454,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
         <v>43</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
         <v>1234567890</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1554,7 +1554,7 @@
         <v>51</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1574,7 +1574,7 @@
         <v>41</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1594,7 +1594,7 @@
         <v>43</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1676,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1696,7 +1696,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1716,7 +1716,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1736,7 +1736,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1756,7 +1756,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1776,7 +1776,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,7 +1816,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1836,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1876,7 +1876,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,7 +1896,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,7 +1916,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1956,7 +1956,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,7 +1976,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,7 +1996,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2016,7 +2016,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2056,7 +2056,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2116,7 +2116,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2136,7 +2136,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2176,7 +2176,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2196,7 +2196,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2236,7 +2236,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2296,7 +2296,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2316,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2356,7 +2356,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2376,7 +2376,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2396,7 +2396,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2416,7 +2416,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2436,7 +2436,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2476,7 +2476,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2496,7 +2496,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2516,7 +2516,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2536,7 +2536,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2556,7 +2556,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2569,7 +2569,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2596,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2616,7 +2616,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2656,7 +2656,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2676,7 +2676,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2696,7 +2696,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2716,7 +2716,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2736,7 +2736,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2756,7 +2756,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2776,7 +2776,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2796,7 +2796,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2816,7 +2816,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2856,7 +2856,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2896,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2916,7 +2916,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2936,7 +2936,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2956,7 +2956,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2976,7 +2976,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2996,7 +2996,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3016,7 +3016,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3036,7 +3036,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3056,7 +3056,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3076,7 +3076,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -3096,7 +3096,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3116,7 +3116,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -3136,7 +3136,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -3156,7 +3156,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3216,7 +3216,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3236,7 +3236,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3256,7 +3256,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3276,7 +3276,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3293,15 +3293,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -3316,12 +3316,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -3336,12 +3336,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -3356,12 +3356,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -3373,35 +3373,35 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>84</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -3416,12 +3416,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -3436,7 +3436,7 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3448,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3476,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3496,7 +3496,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3516,7 +3516,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3536,7 +3536,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3556,7 +3556,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3573,10 +3573,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3596,7 +3596,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3616,7 +3616,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3636,7 +3636,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3673,10 +3673,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -3693,10 +3693,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3713,10 +3713,10 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3736,7 +3736,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3756,7 +3756,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3776,7 +3776,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3796,7 +3796,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3816,7 +3816,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3836,7 +3836,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3856,7 +3856,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3876,7 +3876,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3896,7 +3896,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3916,7 +3916,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3936,7 +3936,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3956,7 +3956,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -3976,7 +3976,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3996,7 +3996,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4016,7 +4016,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4036,7 +4036,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4056,7 +4056,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4076,7 +4076,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -4096,7 +4096,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -4116,7 +4116,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -4156,7 +4156,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -4173,15 +4173,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -4196,12 +4196,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -4216,12 +4216,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -4236,12 +4236,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -4253,35 +4253,35 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="b">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>84</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -4296,12 +4296,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -4316,47 +4316,47 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
         <v>91</v>
       </c>
-      <c r="B44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
       <c r="F44" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
         <v>93</v>
       </c>
-      <c r="B45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" t="s">
-        <v>94</v>
-      </c>
       <c r="F45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4369,7 +4369,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4396,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4416,7 +4416,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4436,7 +4436,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4456,7 +4456,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4476,7 +4476,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4493,10 +4493,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4516,7 +4516,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -4536,7 +4536,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4576,7 +4576,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4593,10 +4593,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -4613,10 +4613,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -4633,10 +4633,10 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -4656,7 +4656,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4676,7 +4676,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -4696,7 +4696,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4716,7 +4716,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -4736,7 +4736,7 @@
         <v>39</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -4756,7 +4756,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -4776,7 +4776,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -4796,7 +4796,7 @@
         <v>45</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -4816,7 +4816,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -4836,7 +4836,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4856,7 +4856,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4876,7 +4876,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4896,7 +4896,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -4913,10 +4913,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4936,7 +4936,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4956,7 +4956,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4996,7 +4996,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -5016,7 +5016,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5036,7 +5036,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5056,7 +5056,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -5076,7 +5076,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -5093,15 +5093,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -5116,12 +5116,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -5136,12 +5136,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -5156,12 +5156,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -5173,15 +5173,15 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -5196,12 +5196,12 @@
         <v>72</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -5216,12 +5216,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -5236,52 +5236,52 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
         <v>91</v>
       </c>
-      <c r="B44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
       <c r="F44" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
         <v>93</v>
       </c>
-      <c r="B45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" t="s">
-        <v>94</v>
-      </c>
       <c r="F45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -5296,12 +5296,12 @@
         <v>41</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -5316,7 +5316,7 @@
         <v>63</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5356,7 +5356,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5373,10 +5373,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5396,7 +5396,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5416,7 +5416,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5433,10 +5433,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5453,10 +5453,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -5476,7 +5476,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5496,7 +5496,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -5516,7 +5516,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -5533,10 +5533,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5553,10 +5553,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5573,10 +5573,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -5596,7 +5596,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -5616,12 +5616,12 @@
         <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -5636,12 +5636,12 @@
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -5653,15 +5653,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -5673,15 +5673,15 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -5696,12 +5696,12 @@
         <v>41</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -5713,15 +5713,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -5736,12 +5736,12 @@
         <v>41</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -5753,15 +5753,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -5773,15 +5773,15 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -5793,15 +5793,15 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -5813,15 +5813,15 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -5833,15 +5833,15 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -5856,12 +5856,12 @@
         <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -5873,15 +5873,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -5896,12 +5896,12 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -5913,15 +5913,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -5933,15 +5933,15 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -5956,12 +5956,12 @@
         <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -5973,10 +5973,10 @@
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5992,7 +5992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61EBF98-981C-4233-B839-BBDDE82D6C34}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -6020,7 +6020,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6037,10 +6037,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6060,7 +6060,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6080,7 +6080,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6097,10 +6097,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6117,10 +6117,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -6140,7 +6140,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -6160,7 +6160,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -6180,7 +6180,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -6197,10 +6197,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -6217,10 +6217,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -6237,10 +6237,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -6260,7 +6260,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -6280,12 +6280,12 @@
         <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -6300,12 +6300,12 @@
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -6317,15 +6317,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -6337,22 +6337,22 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>135</v>
       </c>
-      <c r="B18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>136</v>
-      </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
@@ -6360,12 +6360,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -6377,15 +6377,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -6397,15 +6397,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -6420,12 +6420,12 @@
         <v>41</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -6437,15 +6437,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -6457,15 +6457,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -6477,15 +6477,15 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -6497,15 +6497,15 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -6517,15 +6517,15 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -6537,15 +6537,15 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -6557,15 +6557,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -6580,12 +6580,12 @@
         <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -6597,15 +6597,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -6617,15 +6617,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -6640,12 +6640,12 @@
         <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -6657,15 +6657,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -6677,15 +6677,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -6697,15 +6697,15 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -6720,12 +6720,12 @@
         <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
@@ -6737,15 +6737,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -6757,18 +6757,18 @@
         <v>7</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Draft rsf 2.0.0"
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahi/Developer/ONDC-NTS-Specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9384C-F062-4741-B3A9-6381BD2F36F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C98283-1600-A042-8B96-7554B475E52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settle_misc" sheetId="1" r:id="rId1"/>
@@ -263,6 +263,9 @@
     <t>message.settlement.orders.provider.status</t>
   </si>
   <si>
+    <t>NOT-SETTLED</t>
+  </si>
+  <si>
     <t>message.settlement.orders.provider.reference_no</t>
   </si>
   <si>
@@ -669,9 +672,6 @@
   </si>
   <si>
     <t>2024-05-09</t>
-  </si>
-  <si>
-    <t>NOT_SETTLED</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1214,7 +1214,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1274,7 +1274,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1294,7 +1294,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1314,7 +1314,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1334,7 +1334,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1354,7 +1354,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1374,7 +1374,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1454,7 +1454,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
         <v>43</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
         <v>1234567890</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1554,7 +1554,7 @@
         <v>51</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1574,7 +1574,7 @@
         <v>41</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1594,7 +1594,7 @@
         <v>43</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1676,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1696,7 +1696,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1716,7 +1716,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1736,7 +1736,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1756,7 +1756,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1776,7 +1776,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,7 +1816,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1836,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1876,7 +1876,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,7 +1896,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,7 +1916,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1956,7 +1956,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,7 +1976,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,7 +1996,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2016,7 +2016,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2056,7 +2056,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2096,7 +2096,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2116,7 +2116,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2136,7 +2136,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2176,7 +2176,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2196,7 +2196,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2216,7 +2216,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2236,7 +2236,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2296,7 +2296,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2316,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2356,7 +2356,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2376,7 +2376,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2396,7 +2396,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2416,7 +2416,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2436,7 +2436,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2476,7 +2476,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2496,7 +2496,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2516,7 +2516,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2536,7 +2536,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2556,7 +2556,7 @@
         <v>67</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2569,7 +2569,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2596,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2616,7 +2616,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2636,7 +2636,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2656,7 +2656,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2676,7 +2676,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2696,7 +2696,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2716,7 +2716,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2736,7 +2736,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2756,7 +2756,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2776,7 +2776,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2796,7 +2796,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2816,7 +2816,7 @@
         <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2856,7 +2856,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2896,7 +2896,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2916,7 +2916,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2936,7 +2936,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2956,7 +2956,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2976,7 +2976,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2996,7 +2996,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3016,7 +3016,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3036,7 +3036,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3056,7 +3056,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3076,7 +3076,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -3096,7 +3096,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3116,7 +3116,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -3136,7 +3136,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -3156,7 +3156,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3216,7 +3216,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3236,7 +3236,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3256,7 +3256,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3276,7 +3276,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3293,15 +3293,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -3316,12 +3316,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -3336,12 +3336,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -3356,12 +3356,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -3373,15 +3373,15 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -3393,15 +3393,15 @@
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -3416,12 +3416,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -3436,7 +3436,7 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3448,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3476,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3496,7 +3496,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3516,7 +3516,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3536,7 +3536,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3556,7 +3556,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3573,10 +3573,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3596,7 +3596,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3616,7 +3616,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3636,7 +3636,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3673,10 +3673,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -3693,10 +3693,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3713,10 +3713,10 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3736,7 +3736,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3756,7 +3756,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3776,7 +3776,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3796,7 +3796,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3816,7 +3816,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3836,7 +3836,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3856,7 +3856,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3876,7 +3876,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3896,7 +3896,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3916,7 +3916,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3936,7 +3936,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3956,7 +3956,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -3976,7 +3976,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3996,7 +3996,7 @@
         <v>60</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4016,7 +4016,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4036,7 +4036,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4056,7 +4056,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4076,7 +4076,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -4096,7 +4096,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -4116,7 +4116,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -4156,7 +4156,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -4173,15 +4173,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -4196,12 +4196,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -4216,12 +4216,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -4236,12 +4236,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -4253,15 +4253,15 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -4273,15 +4273,15 @@
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -4296,12 +4296,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -4316,12 +4316,12 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -4333,15 +4333,15 @@
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -4353,10 +4353,10 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4369,7 +4369,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4396,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4416,7 +4416,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4436,7 +4436,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4456,7 +4456,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4476,7 +4476,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4493,10 +4493,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4516,7 +4516,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -4536,7 +4536,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -4576,7 +4576,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4593,10 +4593,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -4613,10 +4613,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -4633,10 +4633,10 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -4656,7 +4656,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4676,7 +4676,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -4696,7 +4696,7 @@
         <v>35</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4716,7 +4716,7 @@
         <v>54</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -4736,7 +4736,7 @@
         <v>39</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -4756,7 +4756,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -4776,7 +4776,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -4796,7 +4796,7 @@
         <v>45</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -4816,7 +4816,7 @@
         <v>57</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -4836,7 +4836,7 @@
         <v>49</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4856,7 +4856,7 @@
         <v>51</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4876,7 +4876,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4896,7 +4896,7 @@
         <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -4913,10 +4913,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4936,7 +4936,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4956,7 +4956,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
         <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4996,7 +4996,7 @@
         <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -5016,7 +5016,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5036,7 +5036,7 @@
         <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5056,7 +5056,7 @@
         <v>74</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -5076,7 +5076,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -5093,15 +5093,15 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -5116,12 +5116,12 @@
         <v>72</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -5136,12 +5136,12 @@
         <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -5156,12 +5156,12 @@
         <v>76</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -5173,15 +5173,15 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" t="b">
         <v>1</v>
@@ -5196,12 +5196,12 @@
         <v>72</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" t="b">
         <v>1</v>
@@ -5216,12 +5216,12 @@
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" t="b">
         <v>1</v>
@@ -5236,12 +5236,12 @@
         <v>76</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" t="b">
         <v>1</v>
@@ -5253,15 +5253,15 @@
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" t="b">
         <v>1</v>
@@ -5273,15 +5273,15 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B46" t="b">
         <v>1</v>
@@ -5296,12 +5296,12 @@
         <v>41</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -5316,7 +5316,7 @@
         <v>63</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -5356,7 +5356,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5373,10 +5373,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5396,7 +5396,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5416,7 +5416,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5433,10 +5433,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5453,10 +5453,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -5476,7 +5476,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5496,7 +5496,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -5516,7 +5516,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -5533,10 +5533,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5553,10 +5553,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5573,10 +5573,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -5596,7 +5596,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -5616,12 +5616,12 @@
         <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -5636,12 +5636,12 @@
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -5653,15 +5653,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -5673,15 +5673,15 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -5696,12 +5696,12 @@
         <v>41</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -5713,15 +5713,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -5736,12 +5736,12 @@
         <v>41</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -5753,15 +5753,15 @@
         <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -5773,15 +5773,15 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -5793,15 +5793,15 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -5813,15 +5813,15 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -5833,15 +5833,15 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
@@ -5856,12 +5856,12 @@
         <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -5873,15 +5873,15 @@
         <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
@@ -5896,12 +5896,12 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -5913,15 +5913,15 @@
         <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -5933,15 +5933,15 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -5956,12 +5956,12 @@
         <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -5973,10 +5973,10 @@
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5992,7 +5992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61EBF98-981C-4233-B839-BBDDE82D6C34}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -6020,7 +6020,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6037,10 +6037,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6060,7 +6060,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6080,7 +6080,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6097,10 +6097,10 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6117,10 +6117,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -6140,7 +6140,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -6160,7 +6160,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -6180,7 +6180,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -6197,10 +6197,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -6217,10 +6217,10 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -6237,10 +6237,10 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -6260,7 +6260,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -6280,12 +6280,12 @@
         <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -6300,12 +6300,12 @@
         <v>41</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -6317,15 +6317,15 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -6337,21 +6337,21 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -6360,12 +6360,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -6377,15 +6377,15 @@
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -6397,15 +6397,15 @@
         <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -6420,12 +6420,12 @@
         <v>41</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -6437,15 +6437,15 @@
         <v>7</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -6457,15 +6457,15 @@
         <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -6477,15 +6477,15 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -6497,15 +6497,15 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -6517,15 +6517,15 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -6537,15 +6537,15 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -6557,15 +6557,15 @@
         <v>7</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -6580,12 +6580,12 @@
         <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -6597,15 +6597,15 @@
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -6617,15 +6617,15 @@
         <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -6640,12 +6640,12 @@
         <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -6657,15 +6657,15 @@
         <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -6677,15 +6677,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -6697,15 +6697,15 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -6720,12 +6720,12 @@
         <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
@@ -6737,15 +6737,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -6757,18 +6757,18 @@
         <v>7</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>